<commit_message>
Show list of updated inventory entries
</commit_message>
<xml_diff>
--- a/src/Files/WorkOrders/160A110V.xlsx
+++ b/src/Files/WorkOrders/160A110V.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke\eclipse-workspace\BURIN_V2\src\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke\eclipse-workspace\BURIN_V2\src\Files\WorkOrders\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -979,7 +979,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A10" sqref="A10:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>

</xml_diff>